<commit_message>
replace wifi model with CSIModel
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14897"/>
+    <workbookView windowWidth="16457" windowHeight="14751"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>seed</t>
   </si>
@@ -51,6 +51,9 @@
     <t>board</t>
   </si>
   <si>
+    <t>3407(k=8)</t>
+  </si>
+  <si>
     <t>desk</t>
   </si>
   <si>
@@ -67,7 +70,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +96,6 @@
       <color rgb="FFFF0000"/>
       <name val="华文细黑"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -603,48 +599,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -654,101 +653,98 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -761,9 +757,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,15 +766,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,12 +776,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,8 +1128,8 @@
   <sheetPr/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1" outlineLevelCol="7"/>
@@ -1156,6 +1137,7 @@
     <col min="1" max="1" width="12.4954954954955" customWidth="1"/>
     <col min="2" max="2" width="14.9189189189189" customWidth="1"/>
     <col min="3" max="3" width="10.045045045045" customWidth="1"/>
+    <col min="5" max="5" width="10.963963963964" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:8">
@@ -1183,13 +1165,13 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>233</v>
       </c>
       <c r="F2" s="1">
@@ -1203,33 +1185,33 @@
       </c>
     </row>
     <row r="3" ht="16.25" spans="1:8">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="16.25" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="16.25" spans="1:8">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>233</v>
       </c>
       <c r="F5" s="1">
@@ -1241,103 +1223,103 @@
       </c>
     </row>
     <row r="6" ht="16.25" spans="1:8">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" ht="16.25" spans="1:8">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" ht="16.25" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" ht="16.25" spans="1:8">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" ht="16.25" spans="1:8">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" ht="16.25" spans="1:8">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" ht="16.25" spans="1:8">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" ht="16.25" spans="1:8">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" ht="21" spans="1:8">
-      <c r="A14" s="7"/>
+    <row r="14" ht="16.25" spans="1:8">
+      <c r="A14" s="6"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>250</v>
       </c>
       <c r="F14" s="1">
@@ -1346,12 +1328,12 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" ht="21" spans="1:8">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="6">
+    <row r="15" ht="16.25" spans="1:8">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5">
         <v>3407</v>
       </c>
       <c r="F15" s="1">
@@ -1364,24 +1346,24 @@
         <v>96.875</v>
       </c>
     </row>
-    <row r="16" ht="21" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="6"/>
+    <row r="16" ht="16.25" spans="1:8">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" ht="16.25" spans="1:8">
-      <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="5" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>233</v>
       </c>
       <c r="F17" s="1">
@@ -1395,11 +1377,11 @@
       </c>
     </row>
     <row r="18" ht="16.25" spans="1:8">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="6">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5">
         <v>3407</v>
       </c>
       <c r="F18" s="1">
@@ -1411,25 +1393,31 @@
       </c>
     </row>
     <row r="19" ht="16.25" spans="1:8">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>100</v>
+      </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>94.271</v>
+      </c>
     </row>
     <row r="20" ht="16.25" spans="1:8">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>233</v>
       </c>
       <c r="F20" s="1">
@@ -1443,11 +1431,11 @@
       </c>
     </row>
     <row r="21" ht="16.25" spans="1:8">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5">
         <v>200</v>
       </c>
       <c r="F21" s="1">
@@ -1461,11 +1449,11 @@
       </c>
     </row>
     <row r="22" ht="16.25" spans="1:8">
-      <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5">
         <v>150</v>
       </c>
       <c r="F22" s="1">
@@ -1479,13 +1467,13 @@
       </c>
     </row>
     <row r="23" ht="16.25" spans="1:8">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>233</v>
       </c>
       <c r="F23" s="1">
@@ -1499,11 +1487,11 @@
       </c>
     </row>
     <row r="24" ht="16.25" spans="1:8">
-      <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5">
         <v>200</v>
       </c>
       <c r="F24" s="1">
@@ -1517,11 +1505,11 @@
       </c>
     </row>
     <row r="25" ht="16.25" spans="1:8">
-      <c r="A25" s="7"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5">
         <v>190</v>
       </c>
       <c r="F25" s="1"/>
@@ -1533,11 +1521,11 @@
       </c>
     </row>
     <row r="26" ht="16.25" spans="1:8">
-      <c r="A26" s="7"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5">
         <v>180</v>
       </c>
       <c r="F26" s="1"/>
@@ -1549,11 +1537,11 @@
       </c>
     </row>
     <row r="27" ht="16.25" spans="1:8">
-      <c r="A27" s="7"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5">
         <v>170</v>
       </c>
       <c r="F27" s="1"/>
@@ -1565,11 +1553,11 @@
       </c>
     </row>
     <row r="28" ht="16.25" spans="1:8">
-      <c r="A28" s="7"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5">
         <v>150</v>
       </c>
       <c r="F28" s="1"/>
@@ -1581,11 +1569,11 @@
       </c>
     </row>
     <row r="29" ht="16.25" spans="1:8">
-      <c r="A29" s="7"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5">
         <v>100</v>
       </c>
       <c r="F29" s="1"/>
@@ -1595,11 +1583,11 @@
       </c>
     </row>
     <row r="30" ht="16.25" spans="1:8">
-      <c r="A30" s="7"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5">
         <v>50</v>
       </c>
       <c r="F30" s="1"/>
@@ -1609,11 +1597,11 @@
       </c>
     </row>
     <row r="31" ht="16.25" spans="1:8">
-      <c r="A31" s="14"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="6">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5">
         <v>20</v>
       </c>
       <c r="F31" s="1"/>
@@ -1624,18 +1612,18 @@
     </row>
     <row r="32" ht="16.25" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <v>10</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>3407</v>
       </c>
       <c r="F32" s="1"/>
@@ -1643,11 +1631,11 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" ht="16.25" spans="1:8">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="6">
+      <c r="A33" s="6"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5">
         <v>3407</v>
       </c>
       <c r="F33" s="1"/>
@@ -1655,11 +1643,11 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" ht="16.25" spans="1:8">
-      <c r="A34" s="7"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="6">
+      <c r="A34" s="6"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5">
         <v>3407</v>
       </c>
       <c r="F34" s="1"/>
@@ -1667,13 +1655,13 @@
       <c r="H34" s="1"/>
     </row>
     <row r="35" ht="16.25" spans="1:8">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>3407</v>
       </c>
       <c r="F35" s="1"/>
@@ -1681,11 +1669,11 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" ht="16.25" spans="1:8">
-      <c r="A36" s="7"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="6">
+      <c r="A36" s="6"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5">
         <v>3407</v>
       </c>
       <c r="F36" s="1"/>
@@ -1693,11 +1681,11 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" ht="16.25" spans="1:8">
-      <c r="A37" s="7"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="6">
+      <c r="A37" s="6"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5">
         <v>3407</v>
       </c>
       <c r="F37" s="1"/>
@@ -1705,77 +1693,77 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" ht="16.25" spans="1:8">
-      <c r="A38" s="7"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="15">
+      <c r="A38" s="6"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3">
         <v>100</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>3407</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" ht="21" spans="1:8">
-      <c r="A39" s="7"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="6">
+    <row r="39" ht="16.25" spans="1:8">
+      <c r="A39" s="6"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="5">
         <v>3407</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" ht="21" spans="1:8">
-      <c r="A40" s="7"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="6">
+    <row r="40" ht="16.25" spans="1:8">
+      <c r="A40" s="6"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="5">
         <v>3407</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" ht="21" spans="1:8">
-      <c r="A41" s="7"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="9" t="s">
+    <row r="41" ht="16.25" spans="1:8">
+      <c r="A41" s="6"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>3407</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" ht="21" spans="1:8">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="6">
+    <row r="42" ht="16.25" spans="1:8">
+      <c r="A42" s="6"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="5">
         <v>3407</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" ht="21" spans="1:8">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="6">
+    <row r="43" ht="16.25" spans="1:8">
+      <c r="A43" s="6"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="5">
         <v>3407</v>
       </c>
       <c r="F43" s="1"/>
@@ -1783,15 +1771,15 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" ht="16.25" spans="1:8">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>3407</v>
       </c>
       <c r="F44" s="1"/>
@@ -1799,11 +1787,11 @@
       <c r="H44" s="1"/>
     </row>
     <row r="45" ht="16.25" spans="1:8">
-      <c r="A45" s="7"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="6">
+      <c r="A45" s="6"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5">
         <v>3407</v>
       </c>
       <c r="F45" s="1"/>
@@ -1811,11 +1799,11 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" ht="16.25" spans="1:8">
-      <c r="A46" s="7"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="6">
+      <c r="A46" s="6"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5">
         <v>3407</v>
       </c>
       <c r="F46" s="1"/>
@@ -1823,13 +1811,13 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" ht="16.25" spans="1:8">
-      <c r="A47" s="7"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="5" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>3407</v>
       </c>
       <c r="F47" s="1"/>
@@ -1837,11 +1825,11 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" ht="16.25" spans="1:8">
-      <c r="A48" s="7"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="6">
+      <c r="A48" s="6"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5">
         <v>3407</v>
       </c>
       <c r="F48" s="1"/>
@@ -1849,11 +1837,11 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" ht="16.25" spans="1:8">
-      <c r="A49" s="7"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="6">
+      <c r="A49" s="6"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5">
         <v>3407</v>
       </c>
       <c r="F49" s="1"/>
@@ -1861,17 +1849,17 @@
       <c r="H49" s="1"/>
     </row>
     <row r="50" ht="16.25" spans="1:8">
-      <c r="A50" s="7"/>
+      <c r="A50" s="6"/>
       <c r="B50" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <v>3407</v>
       </c>
       <c r="F50" s="1"/>
@@ -1879,11 +1867,11 @@
       <c r="H50" s="1"/>
     </row>
     <row r="51" ht="16.25" spans="1:8">
-      <c r="A51" s="7"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="6">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="5">
         <v>3407</v>
       </c>
       <c r="F51" s="1"/>
@@ -1891,11 +1879,11 @@
       <c r="H51" s="1"/>
     </row>
     <row r="52" ht="16.25" spans="1:8">
-      <c r="A52" s="7"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="6">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="5">
         <v>3407</v>
       </c>
       <c r="F52" s="1"/>
@@ -1903,25 +1891,27 @@
       <c r="H52" s="1"/>
     </row>
     <row r="53" ht="16.25" spans="1:8">
-      <c r="A53" s="7"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="5" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="5">
         <v>3407</v>
       </c>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="G53" s="1">
+        <v>91.146</v>
+      </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" ht="16.25" spans="1:8">
-      <c r="A54" s="7"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="6">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="5">
         <v>3407</v>
       </c>
       <c r="F54" s="1"/>
@@ -1929,11 +1919,11 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" ht="16.25" spans="1:8">
-      <c r="A55" s="7"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="6">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5">
         <v>3407</v>
       </c>
       <c r="F55" s="1"/>
@@ -1941,15 +1931,15 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" ht="16.25" spans="1:8">
-      <c r="A56" s="7"/>
-      <c r="B56" s="10"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5">
         <v>3407</v>
       </c>
       <c r="F56" s="1"/>
@@ -1957,11 +1947,11 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" ht="16.25" spans="1:8">
-      <c r="A57" s="7"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="6">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5">
         <v>3407</v>
       </c>
       <c r="F57" s="1"/>
@@ -1969,11 +1959,11 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" ht="16.25" spans="1:8">
-      <c r="A58" s="7"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="6">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5">
         <v>3407</v>
       </c>
       <c r="F58" s="1"/>
@@ -1981,13 +1971,13 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" ht="16.25" spans="1:8">
-      <c r="A59" s="7"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5" t="s">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="5">
         <v>3407</v>
       </c>
       <c r="F59" s="1"/>
@@ -1995,11 +1985,11 @@
       <c r="H59" s="1"/>
     </row>
     <row r="60" ht="16.25" spans="1:8">
-      <c r="A60" s="7"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="6">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5">
         <v>3407</v>
       </c>
       <c r="F60" s="1"/>
@@ -2007,11 +1997,11 @@
       <c r="H60" s="1"/>
     </row>
     <row r="61" ht="16.25" spans="1:8">
-      <c r="A61" s="14"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="6">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="5">
         <v>3407</v>
       </c>
       <c r="F61" s="1"/>

</xml_diff>

<commit_message>
update result of LLM
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -910,7 +910,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -942,27 +942,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1334,10 +1313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I209"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="O67" sqref="O67"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
@@ -1980,7 +1959,7 @@
       </c>
     </row>
     <row r="34" ht="16.25" spans="1:8">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2006,7 +1985,7 @@
       </c>
     </row>
     <row r="35" ht="16.25" spans="1:8">
-      <c r="A35" s="11"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="4"/>
@@ -2024,7 +2003,7 @@
       </c>
     </row>
     <row r="36" ht="16.25" spans="1:8">
-      <c r="A36" s="11"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="4"/>
@@ -2042,7 +2021,7 @@
       </c>
     </row>
     <row r="37" ht="16.25" spans="1:8">
-      <c r="A37" s="11"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="4" t="s">
@@ -2062,7 +2041,7 @@
       </c>
     </row>
     <row r="38" ht="16.25" spans="1:8">
-      <c r="A38" s="11"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="4"/>
@@ -2080,7 +2059,7 @@
       </c>
     </row>
     <row r="39" ht="16.25" spans="1:8">
-      <c r="A39" s="11"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="4"/>
@@ -2098,7 +2077,7 @@
       </c>
     </row>
     <row r="40" ht="16.25" spans="1:8">
-      <c r="A40" s="11"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="4"/>
@@ -2116,7 +2095,7 @@
       </c>
     </row>
     <row r="41" ht="16.25" spans="1:8">
-      <c r="A41" s="11"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="4"/>
@@ -2134,7 +2113,7 @@
       </c>
     </row>
     <row r="42" ht="16.25" spans="1:8">
-      <c r="A42" s="11"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="4"/>
@@ -2152,7 +2131,7 @@
       </c>
     </row>
     <row r="43" ht="16.25" spans="1:8">
-      <c r="A43" s="11"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
         <v>100</v>
@@ -2174,7 +2153,7 @@
       </c>
     </row>
     <row r="44" ht="16.25" spans="1:8">
-      <c r="A44" s="11"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="4"/>
@@ -2192,7 +2171,7 @@
       </c>
     </row>
     <row r="45" ht="16.25" spans="1:8">
-      <c r="A45" s="11"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="4"/>
@@ -2210,7 +2189,7 @@
       </c>
     </row>
     <row r="46" ht="16.25" spans="1:8">
-      <c r="A46" s="11"/>
+      <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="4"/>
@@ -2228,7 +2207,7 @@
       </c>
     </row>
     <row r="47" ht="16.25" spans="1:8">
-      <c r="A47" s="11"/>
+      <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="4"/>
@@ -2246,7 +2225,7 @@
       </c>
     </row>
     <row r="48" ht="16.25" spans="1:8">
-      <c r="A48" s="11"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="4"/>
@@ -2264,7 +2243,7 @@
       </c>
     </row>
     <row r="49" ht="16.25" spans="1:8">
-      <c r="A49" s="11"/>
+      <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="4" t="s">
@@ -2284,7 +2263,7 @@
       </c>
     </row>
     <row r="50" ht="16.25" spans="1:8">
-      <c r="A50" s="11"/>
+      <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="4"/>
@@ -2302,7 +2281,7 @@
       </c>
     </row>
     <row r="51" ht="16.25" spans="1:8">
-      <c r="A51" s="11"/>
+      <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="4"/>
@@ -2320,7 +2299,7 @@
       </c>
     </row>
     <row r="52" ht="16.25" spans="1:8">
-      <c r="A52" s="11"/>
+      <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="4"/>
@@ -2338,7 +2317,7 @@
       </c>
     </row>
     <row r="53" ht="16.25" spans="1:8">
-      <c r="A53" s="11"/>
+      <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
         <v>13</v>
@@ -2360,7 +2339,7 @@
       </c>
     </row>
     <row r="54" ht="16.25" spans="1:8">
-      <c r="A54" s="11"/>
+      <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="4"/>
@@ -2378,7 +2357,7 @@
       </c>
     </row>
     <row r="55" ht="16.25" spans="1:8">
-      <c r="A55" s="11"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="4"/>
@@ -2396,7 +2375,7 @@
       </c>
     </row>
     <row r="56" ht="16.25" spans="1:8">
-      <c r="A56" s="11"/>
+      <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="4"/>
@@ -2414,7 +2393,7 @@
       </c>
     </row>
     <row r="57" ht="16.25" spans="1:8">
-      <c r="A57" s="11"/>
+      <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="4"/>
@@ -2432,7 +2411,7 @@
       </c>
     </row>
     <row r="58" ht="16.25" spans="1:8">
-      <c r="A58" s="11"/>
+      <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="4"/>
@@ -2450,7 +2429,7 @@
       </c>
     </row>
     <row r="59" ht="16.25" spans="1:8">
-      <c r="A59" s="11"/>
+      <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="4"/>
@@ -2468,7 +2447,7 @@
       </c>
     </row>
     <row r="60" ht="16.25" spans="1:8">
-      <c r="A60" s="11"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="4" t="s">
@@ -2488,7 +2467,7 @@
       </c>
     </row>
     <row r="61" ht="16.25" spans="1:8">
-      <c r="A61" s="11"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="4"/>
@@ -2506,7 +2485,7 @@
       </c>
     </row>
     <row r="62" ht="16.25" spans="1:8">
-      <c r="A62" s="11"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="4"/>
@@ -2524,7 +2503,7 @@
       </c>
     </row>
     <row r="63" ht="16.25" spans="1:8">
-      <c r="A63" s="11"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="4"/>
@@ -2542,7 +2521,7 @@
       </c>
     </row>
     <row r="64" ht="16.25" spans="1:8">
-      <c r="A64" s="11"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="4"/>
@@ -2560,7 +2539,7 @@
       </c>
     </row>
     <row r="65" ht="16.25" spans="1:8">
-      <c r="A65" s="11"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
         <v>19</v>
       </c>
@@ -2584,7 +2563,7 @@
       </c>
     </row>
     <row r="66" ht="16.25" spans="1:8">
-      <c r="A66" s="11"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="4"/>
@@ -2602,7 +2581,7 @@
       </c>
     </row>
     <row r="67" ht="16.25" spans="1:8">
-      <c r="A67" s="11"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="4"/>
@@ -2620,7 +2599,7 @@
       </c>
     </row>
     <row r="68" ht="16.25" spans="1:8">
-      <c r="A68" s="11"/>
+      <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="4" t="s">
@@ -2640,7 +2619,7 @@
       </c>
     </row>
     <row r="69" ht="16.25" spans="1:8">
-      <c r="A69" s="11"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="4"/>
@@ -2658,7 +2637,7 @@
       </c>
     </row>
     <row r="70" ht="16.25" spans="1:8">
-      <c r="A70" s="11"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="4"/>
@@ -2676,9 +2655,9 @@
       </c>
     </row>
     <row r="71" ht="16.25" spans="1:8">
-      <c r="A71" s="11"/>
+      <c r="A71" s="2"/>
       <c r="B71" s="2"/>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="4" t="s">
@@ -2698,9 +2677,9 @@
       </c>
     </row>
     <row r="72" ht="16.25" spans="1:8">
-      <c r="A72" s="11"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="13"/>
+      <c r="C72" s="3"/>
       <c r="D72" s="4"/>
       <c r="E72" s="5" t="s">
         <v>8</v>
@@ -2716,10 +2695,10 @@
       </c>
     </row>
     <row r="73" ht="16.25" spans="1:8">
-      <c r="A73" s="11"/>
+      <c r="A73" s="2"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="14" t="s">
+      <c r="C73" s="3"/>
+      <c r="D73" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -2736,10 +2715,10 @@
       </c>
     </row>
     <row r="74" ht="16.25" spans="1:8">
-      <c r="A74" s="11"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="2"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="15"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="8"/>
       <c r="E74" s="5" t="s">
         <v>8</v>
       </c>
@@ -2754,10 +2733,10 @@
       </c>
     </row>
     <row r="75" ht="16.25" spans="1:9">
-      <c r="A75" s="11"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="2"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="15"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="8"/>
       <c r="E75" s="5" t="s">
         <v>26</v>
       </c>
@@ -2775,10 +2754,10 @@
       </c>
     </row>
     <row r="76" ht="16.25" spans="1:8">
-      <c r="A76" s="11"/>
+      <c r="A76" s="2"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="15"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="8"/>
       <c r="E76" s="5" t="s">
         <v>28</v>
       </c>
@@ -2793,10 +2772,10 @@
       </c>
     </row>
     <row r="77" ht="16.25" spans="1:8">
-      <c r="A77" s="11"/>
+      <c r="A77" s="2"/>
       <c r="B77" s="2"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="15"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="8"/>
       <c r="E77" s="5" t="s">
         <v>23</v>
       </c>
@@ -2811,10 +2790,10 @@
       </c>
     </row>
     <row r="78" ht="16.25" spans="1:8">
-      <c r="A78" s="11"/>
+      <c r="A78" s="2"/>
       <c r="B78" s="2"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="15"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="8"/>
       <c r="E78" s="5" t="s">
         <v>29</v>
       </c>
@@ -2829,10 +2808,10 @@
       </c>
     </row>
     <row r="79" ht="16.25" spans="1:8">
-      <c r="A79" s="11"/>
+      <c r="A79" s="2"/>
       <c r="B79" s="2"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="15"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="8"/>
       <c r="E79" s="5" t="s">
         <v>9</v>
       </c>
@@ -2847,10 +2826,10 @@
       </c>
     </row>
     <row r="80" ht="16.25" spans="1:8">
-      <c r="A80" s="11"/>
+      <c r="A80" s="2"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="15"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="8"/>
       <c r="E80" s="5" t="s">
         <v>30</v>
       </c>
@@ -2865,10 +2844,10 @@
       </c>
     </row>
     <row r="81" ht="16.25" spans="1:8">
-      <c r="A81" s="11"/>
+      <c r="A81" s="2"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="15"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="8"/>
       <c r="E81" s="5" t="s">
         <v>31</v>
       </c>
@@ -2883,10 +2862,10 @@
       </c>
     </row>
     <row r="82" ht="16.25" spans="1:8">
-      <c r="A82" s="11"/>
+      <c r="A82" s="2"/>
       <c r="B82" s="2"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="15"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="8"/>
       <c r="E82" s="5" t="s">
         <v>32</v>
       </c>
@@ -2901,10 +2880,10 @@
       </c>
     </row>
     <row r="83" ht="16.25" spans="1:8">
-      <c r="A83" s="11"/>
+      <c r="A83" s="2"/>
       <c r="B83" s="2"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="15"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="8"/>
       <c r="E83" s="5" t="s">
         <v>33</v>
       </c>
@@ -2919,10 +2898,10 @@
       </c>
     </row>
     <row r="84" ht="16.25" spans="1:8">
-      <c r="A84" s="11"/>
+      <c r="A84" s="2"/>
       <c r="B84" s="2"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="15"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="8"/>
       <c r="E84" s="5" t="s">
         <v>17</v>
       </c>
@@ -2937,10 +2916,10 @@
       </c>
     </row>
     <row r="85" ht="16.25" spans="1:8">
-      <c r="A85" s="11"/>
+      <c r="A85" s="2"/>
       <c r="B85" s="2"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="15"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="8"/>
       <c r="E85" s="5" t="s">
         <v>34</v>
       </c>
@@ -2955,10 +2934,10 @@
       </c>
     </row>
     <row r="86" ht="16.25" spans="1:8">
-      <c r="A86" s="11"/>
+      <c r="A86" s="2"/>
       <c r="B86" s="2"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="15"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="8"/>
       <c r="E86" s="5" t="s">
         <v>12</v>
       </c>
@@ -2973,10 +2952,10 @@
       </c>
     </row>
     <row r="87" ht="16.25" spans="1:9">
-      <c r="A87" s="11"/>
+      <c r="A87" s="2"/>
       <c r="B87" s="2"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="15"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="8"/>
       <c r="E87" s="5" t="s">
         <v>35</v>
       </c>
@@ -2989,13 +2968,13 @@
       <c r="H87" s="1">
         <v>97.396</v>
       </c>
-      <c r="I87" s="23"/>
+      <c r="I87" s="16"/>
     </row>
     <row r="88" ht="16.25" spans="1:9">
-      <c r="A88" s="11"/>
+      <c r="A88" s="2"/>
       <c r="B88" s="2"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="15"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="8"/>
       <c r="E88" s="5" t="s">
         <v>36</v>
       </c>
@@ -3008,13 +2987,13 @@
       <c r="H88" s="1">
         <v>97.917</v>
       </c>
-      <c r="I88" s="23"/>
+      <c r="I88" s="16"/>
     </row>
     <row r="89" ht="16.25" spans="1:8">
-      <c r="A89" s="11"/>
+      <c r="A89" s="2"/>
       <c r="B89" s="6"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="17"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="9"/>
       <c r="E89" s="5" t="s">
         <v>10</v>
       </c>
@@ -3028,13 +3007,13 @@
         <v>97.396</v>
       </c>
     </row>
-    <row r="90" ht="16.25" spans="1:9">
-      <c r="A90" s="11"/>
-      <c r="B90" s="18" t="s">
+    <row r="90" ht="16.25" spans="1:10">
+      <c r="A90" s="2"/>
+      <c r="B90" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="15" t="s">
+      <c r="C90" s="12"/>
+      <c r="D90" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="5" t="s">
@@ -3045,15 +3024,18 @@
       <c r="H90" s="1">
         <v>97.396</v>
       </c>
-      <c r="I90" s="24" t="s">
+      <c r="I90" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="91" ht="16.25" spans="1:9">
-      <c r="A91" s="11"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="15"/>
+      <c r="J90" s="1">
+        <v>95.833</v>
+      </c>
+    </row>
+    <row r="91" ht="16.25" spans="1:10">
+      <c r="A91" s="2"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="8"/>
       <c r="E91" s="5" t="s">
         <v>7</v>
       </c>
@@ -3062,15 +3044,18 @@
       <c r="H91" s="1">
         <v>86.979</v>
       </c>
-      <c r="I91" s="24" t="s">
+      <c r="I91" s="17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="92" ht="16.25" spans="1:9">
-      <c r="A92" s="11"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="15"/>
+      <c r="J91" s="1">
+        <v>95.833</v>
+      </c>
+    </row>
+    <row r="92" ht="16.25" spans="1:10">
+      <c r="A92" s="2"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="8"/>
       <c r="E92" s="5" t="s">
         <v>7</v>
       </c>
@@ -3079,15 +3064,18 @@
       <c r="H92" s="1">
         <v>75.521</v>
       </c>
-      <c r="I92" s="24">
+      <c r="I92" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" ht="16.25" spans="1:9">
-      <c r="A93" s="11"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="15"/>
+      <c r="J92" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" ht="16.25" spans="1:10">
+      <c r="A93" s="2"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="8"/>
       <c r="E93" s="5" t="s">
         <v>7</v>
       </c>
@@ -3096,15 +3084,18 @@
       <c r="H93" s="1">
         <v>81.771</v>
       </c>
-      <c r="I93" s="24">
+      <c r="I93" s="17">
         <v>100</v>
       </c>
-    </row>
-    <row r="94" ht="16.25" spans="1:9">
-      <c r="A94" s="11"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="17"/>
+      <c r="J93" s="1">
+        <v>96.354</v>
+      </c>
+    </row>
+    <row r="94" ht="16.25" spans="1:10">
+      <c r="A94" s="2"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="9"/>
       <c r="E94" s="5" t="s">
         <v>7</v>
       </c>
@@ -3113,8 +3104,11 @@
       <c r="H94" s="1">
         <v>62.5</v>
       </c>
-      <c r="I94" s="24" t="s">
+      <c r="I94" s="17" t="s">
         <v>13</v>
+      </c>
+      <c r="J94" s="1">
+        <v>93.75</v>
       </c>
     </row>
     <row r="102" ht="21" spans="1:8">
@@ -3151,13 +3145,13 @@
       <c r="E103" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F103" s="22">
+      <c r="F103" s="15">
         <v>85.938</v>
       </c>
-      <c r="G103" s="22">
+      <c r="G103" s="15">
         <v>63.021</v>
       </c>
-      <c r="H103" s="22">
+      <c r="H103" s="15">
         <v>93.229</v>
       </c>
     </row>
@@ -3243,11 +3237,11 @@
       <c r="E108" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F108" s="22">
+      <c r="F108" s="15">
         <v>95.833</v>
       </c>
-      <c r="G108" s="22"/>
-      <c r="H108" s="22">
+      <c r="G108" s="15"/>
+      <c r="H108" s="15">
         <v>92.708</v>
       </c>
     </row>
@@ -3641,11 +3635,11 @@
       <c r="E131" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F131" s="22">
+      <c r="F131" s="15">
         <v>90.625</v>
       </c>
-      <c r="G131" s="22"/>
-      <c r="H131" s="22"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
     </row>
     <row r="132" ht="16.25" spans="1:8">
       <c r="A132" s="3"/>
@@ -3655,13 +3649,13 @@
       <c r="E132" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F132" s="22">
+      <c r="F132" s="15">
         <v>92.188</v>
       </c>
-      <c r="G132" s="22">
+      <c r="G132" s="15">
         <v>88.021</v>
       </c>
-      <c r="H132" s="22">
+      <c r="H132" s="15">
         <v>96.875</v>
       </c>
     </row>
@@ -3693,13 +3687,13 @@
       <c r="E134" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F134" s="22">
+      <c r="F134" s="15">
         <v>98.958</v>
       </c>
-      <c r="G134" s="22">
+      <c r="G134" s="15">
         <v>89.583</v>
       </c>
-      <c r="H134" s="22">
+      <c r="H134" s="15">
         <v>95.833</v>
       </c>
     </row>
@@ -3711,11 +3705,11 @@
       <c r="E135" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F135" s="22">
+      <c r="F135" s="15">
         <v>98.958</v>
       </c>
-      <c r="G135" s="22"/>
-      <c r="H135" s="22">
+      <c r="G135" s="15"/>
+      <c r="H135" s="15">
         <v>95.321</v>
       </c>
     </row>
@@ -3749,13 +3743,13 @@
       <c r="E137" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F137" s="22">
+      <c r="F137" s="15">
         <v>91.667</v>
       </c>
-      <c r="G137" s="22">
+      <c r="G137" s="15">
         <v>76.562</v>
       </c>
-      <c r="H137" s="22">
+      <c r="H137" s="15">
         <v>95.833</v>
       </c>
     </row>
@@ -3767,13 +3761,13 @@
       <c r="E138" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F138" s="22">
+      <c r="F138" s="15">
         <v>89.062</v>
       </c>
-      <c r="G138" s="22">
+      <c r="G138" s="15">
         <v>85.938</v>
       </c>
-      <c r="H138" s="22">
+      <c r="H138" s="15">
         <v>93.75</v>
       </c>
     </row>
@@ -3785,13 +3779,13 @@
       <c r="E139" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F139" s="22">
+      <c r="F139" s="15">
         <v>95.833</v>
       </c>
-      <c r="G139" s="22">
+      <c r="G139" s="15">
         <v>81.25</v>
       </c>
-      <c r="H139" s="22">
+      <c r="H139" s="15">
         <v>94.792</v>
       </c>
     </row>
@@ -3823,13 +3817,13 @@
       <c r="E141" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F141" s="22">
+      <c r="F141" s="15">
         <v>99.479</v>
       </c>
-      <c r="G141" s="22">
+      <c r="G141" s="15">
         <v>76.562</v>
       </c>
-      <c r="H141" s="22">
+      <c r="H141" s="15">
         <v>93.75</v>
       </c>
     </row>
@@ -3841,13 +3835,13 @@
       <c r="E142" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F142" s="22">
+      <c r="F142" s="15">
         <v>100</v>
       </c>
-      <c r="G142" s="22">
+      <c r="G142" s="15">
         <v>85.938</v>
       </c>
-      <c r="H142" s="22">
+      <c r="H142" s="15">
         <v>93.705</v>
       </c>
     </row>
@@ -3859,11 +3853,11 @@
       <c r="E143" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F143" s="22"/>
-      <c r="G143" s="22">
+      <c r="F143" s="15"/>
+      <c r="G143" s="15">
         <v>81.25</v>
       </c>
-      <c r="H143" s="22">
+      <c r="H143" s="15">
         <v>96.354</v>
       </c>
     </row>
@@ -3875,11 +3869,11 @@
       <c r="E144" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F144" s="22"/>
-      <c r="G144" s="22">
+      <c r="F144" s="15"/>
+      <c r="G144" s="15">
         <v>88.021</v>
       </c>
-      <c r="H144" s="22">
+      <c r="H144" s="15">
         <v>94.792</v>
       </c>
     </row>
@@ -3891,11 +3885,11 @@
       <c r="E145" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F145" s="22"/>
-      <c r="G145" s="22">
+      <c r="F145" s="15"/>
+      <c r="G145" s="15">
         <v>86.458</v>
       </c>
-      <c r="H145" s="22">
+      <c r="H145" s="15">
         <v>93.75</v>
       </c>
     </row>
@@ -3907,11 +3901,11 @@
       <c r="E146" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F146" s="22"/>
-      <c r="G146" s="22">
+      <c r="F146" s="15"/>
+      <c r="G146" s="15">
         <v>81.25</v>
       </c>
-      <c r="H146" s="22">
+      <c r="H146" s="15">
         <v>95.312</v>
       </c>
     </row>
@@ -3923,9 +3917,9 @@
       <c r="E147" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F147" s="22"/>
-      <c r="G147" s="22"/>
-      <c r="H147" s="22">
+      <c r="F147" s="15"/>
+      <c r="G147" s="15"/>
+      <c r="H147" s="15">
         <v>93.229</v>
       </c>
     </row>
@@ -3937,9 +3931,9 @@
       <c r="E148" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F148" s="22"/>
-      <c r="G148" s="22"/>
-      <c r="H148" s="22">
+      <c r="F148" s="15"/>
+      <c r="G148" s="15"/>
+      <c r="H148" s="15">
         <v>96.354</v>
       </c>
     </row>
@@ -3951,9 +3945,9 @@
       <c r="E149" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F149" s="22"/>
-      <c r="G149" s="22"/>
-      <c r="H149" s="22">
+      <c r="F149" s="15"/>
+      <c r="G149" s="15"/>
+      <c r="H149" s="15">
         <v>95.833</v>
       </c>
     </row>
@@ -3989,7 +3983,7 @@
       <c r="G151" s="1">
         <v>81.25</v>
       </c>
-      <c r="H151" s="22"/>
+      <c r="H151" s="15"/>
     </row>
     <row r="152" ht="16.25" spans="1:8">
       <c r="A152" s="3"/>

</xml_diff>